<commit_message>
updating the delieverables with segment 3
</commit_message>
<xml_diff>
--- a/deliverables.xlsx
+++ b/deliverables.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eberm\Documents\projects\capstone_greenhouse_emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D63CCC-F32B-47A4-87D8-4755CB2512C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE82B732-082A-4D40-B4E4-0D4E73B848A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{018F19F5-4CC0-4D0D-A8F7-FB8C22E6D7CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{018F19F5-4CC0-4D0D-A8F7-FB8C22E6D7CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Segment 1" sheetId="2" r:id="rId1"/>
     <sheet name="Segment 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Segment 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Segment 3" sheetId="5" r:id="rId3"/>
     <sheet name="Segment 4" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="82">
   <si>
     <t>Presentation:</t>
   </si>
@@ -252,6 +252,39 @@
   </si>
   <si>
     <t>Presentations are drafted in Google Slides</t>
+  </si>
+  <si>
+    <t>All code in the main branch is production-ready.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most code necessary to complete the machine learning portion of the project </t>
+  </si>
+  <si>
+    <t>Link to Google Slides draft presentation</t>
+  </si>
+  <si>
+    <t>Description of the communication protocols has been removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of data preprocessing </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of feature engineering and feature selection, including their decision-making process </t>
+  </si>
+  <si>
+    <t>Description of how they have trained the model thus far, and any additional training that will take place</t>
+  </si>
+  <si>
+    <t>Description of current accuracy score</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least one interactive element </t>
+  </si>
+  <si>
+    <t>The dashboard presents a data story that is logical and easy to follow for someone unfamiliar with the topic. It includes all of the following:</t>
   </si>
 </sst>
 </file>
@@ -298,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +368,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -348,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -392,6 +431,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -712,7 +763,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -722,20 +773,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968111A5-6001-4035-9C69-05804366EC77}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.1328125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="97.86328125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="22.73046875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="14.265625" style="10" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="10"/>
+    <col min="1" max="1" width="34.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="97.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="10" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C1" s="11" t="s">
         <v>63</v>
       </c>
@@ -743,7 +794,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -751,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>2</v>
       </c>
@@ -762,7 +813,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -773,7 +824,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
@@ -784,7 +835,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
@@ -795,7 +846,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
@@ -806,7 +857,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
@@ -817,7 +868,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
@@ -828,7 +879,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
         <v>70</v>
       </c>
@@ -839,7 +890,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
@@ -853,7 +904,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
@@ -864,7 +915,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>53</v>
       </c>
@@ -875,7 +926,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>25</v>
       </c>
@@ -886,7 +937,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>54</v>
       </c>
@@ -897,7 +948,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
         <v>55</v>
       </c>
@@ -908,7 +959,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
         <v>29</v>
       </c>
@@ -919,7 +970,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>30</v>
       </c>
@@ -930,7 +981,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>31</v>
       </c>
@@ -941,7 +992,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>52</v>
       </c>
@@ -955,7 +1006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>57</v>
       </c>
@@ -966,7 +1017,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
@@ -977,7 +1028,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
         <v>36</v>
       </c>
@@ -988,7 +1039,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>51</v>
       </c>
@@ -1002,7 +1053,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
         <v>42</v>
       </c>
@@ -1013,7 +1064,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>43</v>
       </c>
@@ -1024,7 +1075,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
         <v>44</v>
       </c>
@@ -1035,7 +1086,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="7" t="s">
         <v>45</v>
       </c>
@@ -1046,7 +1097,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>58</v>
       </c>
@@ -1057,7 +1108,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>46</v>
       </c>
@@ -1071,7 +1122,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>60</v>
       </c>
@@ -1082,7 +1133,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="7" t="s">
         <v>61</v>
       </c>
@@ -1093,7 +1144,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>62</v>
       </c>
@@ -1111,16 +1162,447 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0930DF13-8150-4AE9-A195-90D169144963}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8A96A5-9D80-461B-B12F-77EACBCED54A}">
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1128,19 +1610,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E53BDDB-3F91-47D8-98BD-957091AD1176}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="114.73046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="2"/>
+    <col min="1" max="1" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="114.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1148,247 +1630,247 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="39.4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="39.4" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
update the readme with dashboard information and update the segment 3 deliverables
</commit_message>
<xml_diff>
--- a/deliverables.xlsx
+++ b/deliverables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eberm\Documents\projects\capstone_greenhouse_emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE82B732-082A-4D40-B4E4-0D4E73B848A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE879C5-BC68-4F65-BC9D-03B29ABC0D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="2" xr2:uid="{018F19F5-4CC0-4D0D-A8F7-FB8C22E6D7CE}"/>
+    <workbookView xWindow="4680" yWindow="1305" windowWidth="16410" windowHeight="11160" activeTab="2" xr2:uid="{018F19F5-4CC0-4D0D-A8F7-FB8C22E6D7CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Segment 1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
   <si>
     <t>Presentation:</t>
   </si>
@@ -331,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +374,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -387,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -443,6 +449,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -774,7 +783,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1165,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8A96A5-9D80-461B-B12F-77EACBCED54A}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1436,12 +1445,10 @@
       <c r="C25" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="D25" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="21"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
@@ -1450,12 +1457,10 @@
       <c r="C26" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="D26" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
@@ -1464,12 +1469,10 @@
       <c r="C27" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="D27" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="21"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
@@ -1478,12 +1481,10 @@
       <c r="C28" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="D28" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="21"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
@@ -1492,12 +1493,10 @@
       <c r="C29" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="D29" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="21"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
@@ -1506,12 +1505,10 @@
       <c r="C30" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="D30" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
@@ -1520,12 +1517,10 @@
       <c r="C31" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>69</v>
-      </c>
+      <c r="D31" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="21"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
@@ -1551,11 +1546,11 @@
       <c r="C35" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>64</v>
+      <c r="D35" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1565,11 +1560,11 @@
       <c r="C36" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>64</v>
+      <c r="D36" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1579,11 +1574,11 @@
       <c r="C37" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>64</v>
+      <c r="D37" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1593,11 +1588,11 @@
       <c r="C38" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D38" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>64</v>
+      <c r="D38" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1610,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E53BDDB-3F91-47D8-98BD-957091AD1176}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1780,82 +1775,85 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B35" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B36" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B37" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B38" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B39" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B40" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B41" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>46</v>
       </c>

</xml_diff>